<commit_message>
Add resource to table
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chelsea/Documents/Microsoft/領袖營/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\GitHub\MSSeed13Camp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23100" windowHeight="15460" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="23100" windowHeight="15465" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
     <sheet name="account" sheetId="2" r:id="rId2"/>
+    <sheet name="resource" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="401">
   <si>
     <t>簡嘉誼</t>
   </si>
@@ -1130,15 +1131,126 @@
   <si>
     <t>(自訂)</t>
   </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t>magic_powder</t>
+  </si>
+  <si>
+    <t>cloth</t>
+  </si>
+  <si>
+    <t>ruby</t>
+  </si>
+  <si>
+    <t>shaft</t>
+  </si>
+  <si>
+    <t>fire</t>
+  </si>
+  <si>
+    <t>seed</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>light</t>
+  </si>
+  <si>
+    <t>flax</t>
+  </si>
+  <si>
+    <t>screw</t>
+  </si>
+  <si>
+    <t>plastic</t>
+  </si>
+  <si>
+    <t>electron</t>
+  </si>
+  <si>
+    <t>ergonomic</t>
+  </si>
+  <si>
+    <t>imagine</t>
+  </si>
+  <si>
+    <t>metal</t>
+  </si>
+  <si>
+    <t>air</t>
+  </si>
+  <si>
+    <t>magic_stone</t>
+  </si>
+  <si>
+    <t>control_panel</t>
+  </si>
+  <si>
+    <t>seat</t>
+  </si>
+  <si>
+    <t>wheel</t>
+  </si>
+  <si>
+    <t>rope</t>
+  </si>
+  <si>
+    <t>cypress</t>
+  </si>
+  <si>
+    <t>propeller</t>
+  </si>
+  <si>
+    <t>door</t>
+  </si>
+  <si>
+    <t>jet</t>
+  </si>
+  <si>
+    <t>gun</t>
+  </si>
+  <si>
+    <t>elk</t>
+  </si>
+  <si>
+    <t>sound</t>
+  </si>
+  <si>
+    <t>sd_card</t>
+  </si>
+  <si>
+    <t>missile</t>
+  </si>
+  <si>
+    <t>miss_air</t>
+  </si>
+  <si>
+    <t>led_light</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1298,8 +1410,33 @@
       <name val="細明體"/>
       <charset val="136"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13.2"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1312,8 +1449,32 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4CAF50"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1674,11 +1835,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1906,6 +2107,34 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1995,6 +2224,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3081,19 +3313,19 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" style="88" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="88" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="59.83203125" style="1" customWidth="1"/>
-    <col min="9" max="254" width="8.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" style="1" customWidth="1"/>
+    <col min="9" max="254" width="8.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15" customHeight="1">
       <c r="A1" s="88" t="s">
         <v>361</v>
       </c>
@@ -3116,7 +3348,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="88">
         <v>1</v>
       </c>
@@ -3139,7 +3371,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="88">
         <v>2</v>
       </c>
@@ -3162,7 +3394,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="88">
         <v>3</v>
       </c>
@@ -3185,7 +3417,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="88">
         <v>4</v>
       </c>
@@ -3208,7 +3440,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="88">
         <v>5</v>
       </c>
@@ -3231,7 +3463,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="88">
         <v>6</v>
       </c>
@@ -3254,7 +3486,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="88">
         <v>7</v>
       </c>
@@ -3277,7 +3509,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="88">
         <v>8</v>
       </c>
@@ -3300,7 +3532,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="88">
         <v>9</v>
       </c>
@@ -3323,7 +3555,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="88">
         <v>10</v>
       </c>
@@ -3346,7 +3578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="88">
         <v>11</v>
       </c>
@@ -3369,7 +3601,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="88">
         <v>12</v>
       </c>
@@ -3392,7 +3624,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="88">
         <v>13</v>
       </c>
@@ -3415,7 +3647,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="88">
         <v>14</v>
       </c>
@@ -3438,7 +3670,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="88">
         <v>15</v>
       </c>
@@ -3461,7 +3693,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A17" s="88">
         <v>16</v>
       </c>
@@ -3484,7 +3716,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A18" s="88">
         <v>17</v>
       </c>
@@ -3507,7 +3739,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="88">
         <v>18</v>
       </c>
@@ -3530,7 +3762,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="88">
         <v>19</v>
       </c>
@@ -3553,7 +3785,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="88">
         <v>20</v>
       </c>
@@ -3576,7 +3808,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="88">
         <v>21</v>
       </c>
@@ -3599,7 +3831,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="88">
         <v>22</v>
       </c>
@@ -3620,7 +3852,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="88">
         <v>23</v>
       </c>
@@ -3643,7 +3875,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="88">
         <v>24</v>
       </c>
@@ -3666,7 +3898,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="88">
         <v>25</v>
       </c>
@@ -3689,7 +3921,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="88">
         <v>26</v>
       </c>
@@ -3712,7 +3944,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A28" s="88">
         <v>27</v>
       </c>
@@ -3735,7 +3967,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A29" s="88">
         <v>28</v>
       </c>
@@ -3758,7 +3990,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A30" s="88">
         <v>29</v>
       </c>
@@ -3781,7 +4013,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A31" s="88">
         <v>30</v>
       </c>
@@ -3804,7 +4036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A32" s="88">
         <v>31</v>
       </c>
@@ -3827,7 +4059,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A33" s="88">
         <v>32</v>
       </c>
@@ -3850,7 +4082,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A34" s="88">
         <v>33</v>
       </c>
@@ -3873,7 +4105,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A35" s="88">
         <v>34</v>
       </c>
@@ -3896,7 +4128,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A36" s="88">
         <v>35</v>
       </c>
@@ -3919,7 +4151,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A37" s="88">
         <v>36</v>
       </c>
@@ -3942,7 +4174,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A38" s="88">
         <v>37</v>
       </c>
@@ -3965,7 +4197,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A39" s="88">
         <v>38</v>
       </c>
@@ -3988,7 +4220,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A40" s="88">
         <v>39</v>
       </c>
@@ -4011,7 +4243,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A41" s="88">
         <v>40</v>
       </c>
@@ -4034,7 +4266,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A42" s="88">
         <v>41</v>
       </c>
@@ -4057,7 +4289,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A43" s="88">
         <v>42</v>
       </c>
@@ -4080,7 +4312,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A44" s="88">
         <v>43</v>
       </c>
@@ -4103,7 +4335,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A45" s="88">
         <v>44</v>
       </c>
@@ -4126,7 +4358,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A46" s="88">
         <v>45</v>
       </c>
@@ -4149,7 +4381,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A47" s="88">
         <v>46</v>
       </c>
@@ -4172,7 +4404,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A48" s="88">
         <v>47</v>
       </c>
@@ -4195,7 +4427,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A49" s="88">
         <v>48</v>
       </c>
@@ -4218,7 +4450,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A50" s="88">
         <v>49</v>
       </c>
@@ -4241,7 +4473,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A51" s="88">
         <v>50</v>
       </c>
@@ -4264,7 +4496,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A52" s="88">
         <v>51</v>
       </c>
@@ -4287,7 +4519,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A53" s="88">
         <v>52</v>
       </c>
@@ -4310,7 +4542,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A54" s="88">
         <v>53</v>
       </c>
@@ -4333,7 +4565,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A55" s="88">
         <v>54</v>
       </c>
@@ -4356,7 +4588,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A56" s="88">
         <v>55</v>
       </c>
@@ -4379,7 +4611,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A57" s="88">
         <v>56</v>
       </c>
@@ -4402,7 +4634,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A58" s="88">
         <v>57</v>
       </c>
@@ -4425,7 +4657,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A59" s="88">
         <v>58</v>
       </c>
@@ -4448,7 +4680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A60" s="88">
         <v>59</v>
       </c>
@@ -4471,7 +4703,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A61" s="88">
         <v>60</v>
       </c>
@@ -4494,7 +4726,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A62" s="88">
         <v>61</v>
       </c>
@@ -4517,7 +4749,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A63" s="88">
         <v>62</v>
       </c>
@@ -4540,7 +4772,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A64" s="88">
         <v>63</v>
       </c>
@@ -4563,7 +4795,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A65" s="88">
         <v>64</v>
       </c>
@@ -4586,7 +4818,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A66" s="88">
         <v>65</v>
       </c>
@@ -4609,7 +4841,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A67" s="88">
         <v>66</v>
       </c>
@@ -4630,7 +4862,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A68" s="88">
         <v>67</v>
       </c>
@@ -4653,7 +4885,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A69" s="88">
         <v>68</v>
       </c>
@@ -4676,7 +4908,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A70" s="88">
         <v>69</v>
       </c>
@@ -4699,7 +4931,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A71" s="88">
         <v>70</v>
       </c>
@@ -4722,7 +4954,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A72" s="88">
         <v>71</v>
       </c>
@@ -4745,7 +4977,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A73" s="88">
         <v>72</v>
       </c>
@@ -4768,7 +5000,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A74" s="88">
         <v>73</v>
       </c>
@@ -4791,7 +5023,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A75" s="88">
         <v>74</v>
       </c>
@@ -4814,7 +5046,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A76" s="88">
         <v>75</v>
       </c>
@@ -4835,7 +5067,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A77" s="88">
         <v>76</v>
       </c>
@@ -4858,7 +5090,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A78" s="88">
         <v>77</v>
       </c>
@@ -4881,7 +5113,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A79" s="88">
         <v>78</v>
       </c>
@@ -4904,7 +5136,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A80" s="88">
         <v>79</v>
       </c>
@@ -4927,7 +5159,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A81" s="88">
         <v>80</v>
       </c>
@@ -4950,7 +5182,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A82" s="88">
         <v>81</v>
       </c>
@@ -4973,7 +5205,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A83" s="88">
         <v>82</v>
       </c>
@@ -4996,7 +5228,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A84" s="88">
         <v>83</v>
       </c>
@@ -5019,7 +5251,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A85" s="88">
         <v>84</v>
       </c>
@@ -5042,7 +5274,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A86" s="88">
         <v>85</v>
       </c>
@@ -5065,7 +5297,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A87" s="88">
         <v>86</v>
       </c>
@@ -5088,7 +5320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A88" s="88">
         <v>87</v>
       </c>
@@ -5111,7 +5343,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A89" s="88">
         <v>88</v>
       </c>
@@ -5134,7 +5366,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A90" s="88">
         <v>89</v>
       </c>
@@ -5157,7 +5389,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A91" s="88">
         <v>90</v>
       </c>
@@ -5180,7 +5412,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A92" s="88">
         <v>91</v>
       </c>
@@ -5203,7 +5435,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A93" s="88">
         <v>92</v>
       </c>
@@ -5226,7 +5458,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A94" s="88">
         <v>93</v>
       </c>
@@ -5249,7 +5481,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A95" s="88">
         <v>94</v>
       </c>
@@ -5272,7 +5504,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A96" s="88">
         <v>95</v>
       </c>
@@ -5295,7 +5527,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A97" s="88">
         <v>96</v>
       </c>
@@ -5318,7 +5550,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A98" s="88">
         <v>97</v>
       </c>
@@ -5341,7 +5573,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A99" s="88">
         <v>98</v>
       </c>
@@ -5364,7 +5596,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A100" s="88">
         <v>99</v>
       </c>
@@ -5387,7 +5619,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A101" s="88">
         <v>100</v>
       </c>
@@ -5410,7 +5642,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A102" s="88">
         <v>101</v>
       </c>
@@ -5433,7 +5665,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A103" s="88">
         <v>102</v>
       </c>
@@ -5456,7 +5688,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A104" s="88">
         <v>103</v>
       </c>
@@ -5479,7 +5711,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A105" s="88">
         <v>104</v>
       </c>
@@ -5520,17 +5752,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="88"/>
-    <col min="2" max="2" width="59.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="88"/>
+    <col min="2" max="2" width="59.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="88" t="s">
         <v>348</v>
       </c>
@@ -5541,7 +5773,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17.25">
       <c r="A2" s="88">
         <v>1</v>
       </c>
@@ -5552,7 +5784,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17.25">
       <c r="A3" s="88">
         <v>2</v>
       </c>
@@ -5560,7 +5792,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17.25">
       <c r="A4" s="88">
         <v>3</v>
       </c>
@@ -5568,7 +5800,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17.25">
       <c r="A5" s="88">
         <v>4</v>
       </c>
@@ -5576,7 +5808,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17.25">
       <c r="A6" s="88">
         <v>5</v>
       </c>
@@ -5584,7 +5816,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="17.25">
       <c r="A7" s="88">
         <v>6</v>
       </c>
@@ -5592,7 +5824,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="17.25">
       <c r="A8" s="88">
         <v>7</v>
       </c>
@@ -5600,7 +5832,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="17.25">
       <c r="A9" s="88">
         <v>8</v>
       </c>
@@ -5608,7 +5840,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="17.25">
       <c r="A10" s="88">
         <v>9</v>
       </c>
@@ -5616,7 +5848,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="17.25">
       <c r="A11" s="88">
         <v>10</v>
       </c>
@@ -5624,7 +5856,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="17.25">
       <c r="A12" s="88">
         <v>11</v>
       </c>
@@ -5632,7 +5864,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="17.25">
       <c r="A13" s="88">
         <v>12</v>
       </c>
@@ -5640,7 +5872,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="17.25">
       <c r="A14" s="88">
         <v>13</v>
       </c>
@@ -5648,7 +5880,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="17.25">
       <c r="A15" s="88">
         <v>14</v>
       </c>
@@ -5656,7 +5888,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="17.25">
       <c r="A16" s="88">
         <v>15</v>
       </c>
@@ -5664,7 +5896,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="17.25">
       <c r="A17" s="88">
         <v>16</v>
       </c>
@@ -5672,7 +5904,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="17.25">
       <c r="A18" s="88">
         <v>17</v>
       </c>
@@ -5680,7 +5912,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="17.25">
       <c r="A19" s="88">
         <v>18</v>
       </c>
@@ -5688,7 +5920,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="17.25">
       <c r="A20" s="88">
         <v>19</v>
       </c>
@@ -5696,7 +5928,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="17.25">
       <c r="A21" s="88">
         <v>20</v>
       </c>
@@ -5704,7 +5936,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" ht="17.25">
       <c r="A22" s="88">
         <v>21</v>
       </c>
@@ -5712,7 +5944,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" ht="17.25">
       <c r="A23" s="88">
         <v>22</v>
       </c>
@@ -5720,7 +5952,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" ht="17.25">
       <c r="A24" s="88">
         <v>23</v>
       </c>
@@ -5728,7 +5960,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" ht="17.25">
       <c r="A25" s="88">
         <v>24</v>
       </c>
@@ -5736,7 +5968,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" ht="17.25">
       <c r="A26" s="88">
         <v>25</v>
       </c>
@@ -5744,7 +5976,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" ht="17.25">
       <c r="A27" s="88">
         <v>26</v>
       </c>
@@ -5752,7 +5984,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" ht="17.25">
       <c r="A28" s="88">
         <v>27</v>
       </c>
@@ -5760,7 +5992,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" ht="17.25">
       <c r="A29" s="88">
         <v>28</v>
       </c>
@@ -5768,7 +6000,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" ht="17.25">
       <c r="A30" s="88">
         <v>29</v>
       </c>
@@ -5776,7 +6008,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" ht="17.25">
       <c r="A31" s="88">
         <v>30</v>
       </c>
@@ -5784,7 +6016,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" ht="17.25">
       <c r="A32" s="88">
         <v>31</v>
       </c>
@@ -5792,7 +6024,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" ht="17.25">
       <c r="A33" s="88">
         <v>32</v>
       </c>
@@ -5800,7 +6032,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" ht="17.25">
       <c r="A34" s="88">
         <v>33</v>
       </c>
@@ -5808,7 +6040,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" ht="17.25">
       <c r="A35" s="88">
         <v>34</v>
       </c>
@@ -5816,7 +6048,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" ht="17.25">
       <c r="A36" s="88">
         <v>35</v>
       </c>
@@ -5824,7 +6056,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" ht="17.25">
       <c r="A37" s="88">
         <v>36</v>
       </c>
@@ -5832,7 +6064,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" ht="17.25">
       <c r="A38" s="88">
         <v>37</v>
       </c>
@@ -5840,7 +6072,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" ht="17.25">
       <c r="A39" s="88">
         <v>38</v>
       </c>
@@ -5848,7 +6080,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" ht="17.25">
       <c r="A40" s="88">
         <v>39</v>
       </c>
@@ -5856,7 +6088,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" ht="17.25">
       <c r="A41" s="88">
         <v>40</v>
       </c>
@@ -5864,7 +6096,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" ht="17.25">
       <c r="A42" s="88">
         <v>41</v>
       </c>
@@ -5872,7 +6104,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" ht="17.25">
       <c r="A43" s="88">
         <v>42</v>
       </c>
@@ -5880,7 +6112,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" ht="17.25">
       <c r="A44" s="88">
         <v>43</v>
       </c>
@@ -5888,7 +6120,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" ht="17.25">
       <c r="A45" s="88">
         <v>44</v>
       </c>
@@ -5896,7 +6128,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" ht="17.25">
       <c r="A46" s="88">
         <v>45</v>
       </c>
@@ -5904,7 +6136,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" ht="17.25">
       <c r="A47" s="88">
         <v>46</v>
       </c>
@@ -5912,7 +6144,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" ht="17.25">
       <c r="A48" s="88">
         <v>47</v>
       </c>
@@ -5920,7 +6152,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" ht="17.25">
       <c r="A49" s="88">
         <v>48</v>
       </c>
@@ -5928,7 +6160,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" ht="17.25">
       <c r="A50" s="88">
         <v>49</v>
       </c>
@@ -5936,7 +6168,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" ht="17.25">
       <c r="A51" s="88">
         <v>50</v>
       </c>
@@ -5944,7 +6176,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" ht="17.25">
       <c r="A52" s="88">
         <v>51</v>
       </c>
@@ -5952,7 +6184,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" ht="17.25">
       <c r="A53" s="88">
         <v>52</v>
       </c>
@@ -5960,7 +6192,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" ht="17.25">
       <c r="A54" s="88">
         <v>53</v>
       </c>
@@ -5968,7 +6200,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" ht="17.25">
       <c r="A55" s="88">
         <v>54</v>
       </c>
@@ -5976,7 +6208,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" ht="17.25">
       <c r="A56" s="88">
         <v>55</v>
       </c>
@@ -5984,7 +6216,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" ht="17.25">
       <c r="A57" s="88">
         <v>56</v>
       </c>
@@ -5992,7 +6224,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" ht="17.25">
       <c r="A58" s="88">
         <v>57</v>
       </c>
@@ -6000,7 +6232,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" ht="17.25">
       <c r="A59" s="88">
         <v>58</v>
       </c>
@@ -6008,7 +6240,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" ht="17.25">
       <c r="A60" s="88">
         <v>59</v>
       </c>
@@ -6016,7 +6248,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" ht="17.25">
       <c r="A61" s="88">
         <v>60</v>
       </c>
@@ -6024,7 +6256,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" ht="17.25">
       <c r="A62" s="88">
         <v>61</v>
       </c>
@@ -6032,7 +6264,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2">
       <c r="A63" s="88">
         <v>62</v>
       </c>
@@ -6040,7 +6272,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" ht="17.25">
       <c r="A64" s="88">
         <v>63</v>
       </c>
@@ -6048,7 +6280,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" ht="17.25">
       <c r="A65" s="88">
         <v>64</v>
       </c>
@@ -6056,7 +6288,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" ht="17.25">
       <c r="A66" s="88">
         <v>65</v>
       </c>
@@ -6064,7 +6296,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" ht="17.25">
       <c r="A67" s="88">
         <v>66</v>
       </c>
@@ -6072,7 +6304,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" ht="17.25">
       <c r="A68" s="88">
         <v>67</v>
       </c>
@@ -6080,7 +6312,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" ht="17.25">
       <c r="A69" s="88">
         <v>68</v>
       </c>
@@ -6088,7 +6320,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" ht="17.25">
       <c r="A70" s="88">
         <v>69</v>
       </c>
@@ -6096,7 +6328,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" ht="17.25">
       <c r="A71" s="88">
         <v>70</v>
       </c>
@@ -6104,7 +6336,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" ht="17.25">
       <c r="A72" s="88">
         <v>71</v>
       </c>
@@ -6112,7 +6344,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" ht="17.25">
       <c r="A73" s="88">
         <v>72</v>
       </c>
@@ -6120,7 +6352,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" ht="17.25">
       <c r="A74" s="88">
         <v>73</v>
       </c>
@@ -6128,7 +6360,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" ht="17.25">
       <c r="A75" s="88">
         <v>74</v>
       </c>
@@ -6136,13 +6368,13 @@
         <v>257</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" ht="17.25">
       <c r="A76" s="88">
         <v>75</v>
       </c>
       <c r="B76" s="29"/>
     </row>
-    <row r="77" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" ht="17.25">
       <c r="A77" s="88">
         <v>76</v>
       </c>
@@ -6150,7 +6382,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" ht="17.25">
       <c r="A78" s="88">
         <v>77</v>
       </c>
@@ -6158,7 +6390,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" ht="17.25">
       <c r="A79" s="88">
         <v>78</v>
       </c>
@@ -6166,7 +6398,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" ht="17.25">
       <c r="A80" s="88">
         <v>79</v>
       </c>
@@ -6174,7 +6406,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" ht="17.25">
       <c r="A81" s="88">
         <v>80</v>
       </c>
@@ -6182,7 +6414,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" ht="17.25">
       <c r="A82" s="88">
         <v>81</v>
       </c>
@@ -6190,7 +6422,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" ht="17.25">
       <c r="A83" s="88">
         <v>82</v>
       </c>
@@ -6198,7 +6430,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" ht="17.25">
       <c r="A84" s="88">
         <v>83</v>
       </c>
@@ -6206,7 +6438,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" ht="17.25">
       <c r="A85" s="88">
         <v>84</v>
       </c>
@@ -6214,7 +6446,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" ht="17.25">
       <c r="A86" s="88">
         <v>85</v>
       </c>
@@ -6222,7 +6454,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" ht="17.25">
       <c r="A87" s="88">
         <v>86</v>
       </c>
@@ -6230,7 +6462,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" ht="17.25">
       <c r="A88" s="88">
         <v>87</v>
       </c>
@@ -6238,7 +6470,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" ht="17.25">
       <c r="A89" s="88">
         <v>88</v>
       </c>
@@ -6246,7 +6478,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" ht="17.25">
       <c r="A90" s="88">
         <v>89</v>
       </c>
@@ -6254,7 +6486,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" ht="17.25">
       <c r="A91" s="88">
         <v>90</v>
       </c>
@@ -6262,7 +6494,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" ht="17.25">
       <c r="A92" s="88">
         <v>91</v>
       </c>
@@ -6270,7 +6502,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" ht="17.25">
       <c r="A93" s="88">
         <v>92</v>
       </c>
@@ -6278,7 +6510,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" ht="17.25">
       <c r="A94" s="88">
         <v>93</v>
       </c>
@@ -6286,7 +6518,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" ht="17.25">
       <c r="A95" s="88">
         <v>94</v>
       </c>
@@ -6294,7 +6526,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" ht="17.25">
       <c r="A96" s="88">
         <v>95</v>
       </c>
@@ -6302,7 +6534,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" ht="17.25">
       <c r="A97" s="88">
         <v>96</v>
       </c>
@@ -6310,7 +6542,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" ht="17.25">
       <c r="A98" s="88">
         <v>97</v>
       </c>
@@ -6318,7 +6550,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" ht="17.25">
       <c r="A99" s="88">
         <v>98</v>
       </c>
@@ -6326,7 +6558,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" ht="17.25">
       <c r="A100" s="88">
         <v>99</v>
       </c>
@@ -6334,7 +6566,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" ht="17.25">
       <c r="A101" s="88">
         <v>100</v>
       </c>
@@ -6342,7 +6574,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" ht="17.25">
       <c r="A102" s="88">
         <v>101</v>
       </c>
@@ -6350,7 +6582,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" ht="17.25">
       <c r="A103" s="88">
         <v>102</v>
       </c>
@@ -6358,7 +6590,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" ht="17.25">
       <c r="A104" s="88">
         <v>103</v>
       </c>
@@ -6366,7 +6598,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" ht="17.25">
       <c r="A105" s="88">
         <v>104</v>
       </c>
@@ -6380,4 +6612,558 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AD10" sqref="AD10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" ht="24.75">
+      <c r="A1" s="91" t="s">
+        <v>368</v>
+      </c>
+      <c r="B1" s="96" t="s">
+        <v>369</v>
+      </c>
+      <c r="C1" s="97" t="s">
+        <v>370</v>
+      </c>
+      <c r="D1" s="96" t="s">
+        <v>371</v>
+      </c>
+      <c r="E1" s="97" t="s">
+        <v>372</v>
+      </c>
+      <c r="F1" s="96" t="s">
+        <v>373</v>
+      </c>
+      <c r="G1" s="97" t="s">
+        <v>374</v>
+      </c>
+      <c r="H1" s="96" t="s">
+        <v>375</v>
+      </c>
+      <c r="I1" s="97" t="s">
+        <v>376</v>
+      </c>
+      <c r="J1" s="96" t="s">
+        <v>377</v>
+      </c>
+      <c r="K1" s="97" t="s">
+        <v>378</v>
+      </c>
+      <c r="L1" s="96" t="s">
+        <v>379</v>
+      </c>
+      <c r="M1" s="97" t="s">
+        <v>380</v>
+      </c>
+      <c r="N1" s="96" t="s">
+        <v>381</v>
+      </c>
+      <c r="O1" s="97" t="s">
+        <v>382</v>
+      </c>
+      <c r="P1" s="96" t="s">
+        <v>383</v>
+      </c>
+      <c r="Q1" s="97" t="s">
+        <v>384</v>
+      </c>
+      <c r="R1" s="96" t="s">
+        <v>385</v>
+      </c>
+      <c r="S1" s="97" t="s">
+        <v>386</v>
+      </c>
+      <c r="T1" s="96" t="s">
+        <v>387</v>
+      </c>
+      <c r="U1" s="97" t="s">
+        <v>388</v>
+      </c>
+      <c r="V1" s="96" t="s">
+        <v>389</v>
+      </c>
+      <c r="W1" s="97" t="s">
+        <v>390</v>
+      </c>
+      <c r="X1" s="96" t="s">
+        <v>391</v>
+      </c>
+      <c r="Y1" s="97" t="s">
+        <v>392</v>
+      </c>
+      <c r="Z1" s="96" t="s">
+        <v>393</v>
+      </c>
+      <c r="AA1" s="97" t="s">
+        <v>394</v>
+      </c>
+      <c r="AB1" s="96" t="s">
+        <v>395</v>
+      </c>
+      <c r="AC1" s="97" t="s">
+        <v>396</v>
+      </c>
+      <c r="AD1" s="96" t="s">
+        <v>397</v>
+      </c>
+      <c r="AE1" s="97" t="s">
+        <v>398</v>
+      </c>
+      <c r="AF1" s="96" t="s">
+        <v>399</v>
+      </c>
+      <c r="AG1" s="98" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" ht="16.5">
+      <c r="A2" s="92" t="s">
+        <v>364</v>
+      </c>
+      <c r="B2" s="89">
+        <v>10</v>
+      </c>
+      <c r="C2" s="89">
+        <v>7</v>
+      </c>
+      <c r="D2" s="89">
+        <v>0</v>
+      </c>
+      <c r="E2" s="89">
+        <v>0</v>
+      </c>
+      <c r="F2" s="89">
+        <v>0</v>
+      </c>
+      <c r="G2" s="89">
+        <v>0</v>
+      </c>
+      <c r="H2" s="89">
+        <v>0</v>
+      </c>
+      <c r="I2" s="89">
+        <v>0</v>
+      </c>
+      <c r="J2" s="89">
+        <v>0</v>
+      </c>
+      <c r="K2" s="89">
+        <v>0</v>
+      </c>
+      <c r="L2" s="89">
+        <v>0</v>
+      </c>
+      <c r="M2" s="89">
+        <v>0</v>
+      </c>
+      <c r="N2" s="89">
+        <v>0</v>
+      </c>
+      <c r="O2" s="89">
+        <v>0</v>
+      </c>
+      <c r="P2" s="89">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="89">
+        <v>0</v>
+      </c>
+      <c r="R2" s="89">
+        <v>0</v>
+      </c>
+      <c r="S2" s="89">
+        <v>0</v>
+      </c>
+      <c r="T2" s="89">
+        <v>0</v>
+      </c>
+      <c r="U2" s="89">
+        <v>0</v>
+      </c>
+      <c r="V2" s="89">
+        <v>0</v>
+      </c>
+      <c r="W2" s="89">
+        <v>0</v>
+      </c>
+      <c r="X2" s="89">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="89">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="89">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="89">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="89">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="89">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="89">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="89">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="89">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="16.5">
+      <c r="A3" s="93" t="s">
+        <v>365</v>
+      </c>
+      <c r="B3" s="90">
+        <v>0</v>
+      </c>
+      <c r="C3" s="90">
+        <v>0</v>
+      </c>
+      <c r="D3" s="90">
+        <v>0</v>
+      </c>
+      <c r="E3" s="90">
+        <v>0</v>
+      </c>
+      <c r="F3" s="90">
+        <v>0</v>
+      </c>
+      <c r="G3" s="90">
+        <v>0</v>
+      </c>
+      <c r="H3" s="90">
+        <v>0</v>
+      </c>
+      <c r="I3" s="90">
+        <v>0</v>
+      </c>
+      <c r="J3" s="90">
+        <v>0</v>
+      </c>
+      <c r="K3" s="90">
+        <v>0</v>
+      </c>
+      <c r="L3" s="90">
+        <v>0</v>
+      </c>
+      <c r="M3" s="90">
+        <v>0</v>
+      </c>
+      <c r="N3" s="90">
+        <v>0</v>
+      </c>
+      <c r="O3" s="90">
+        <v>0</v>
+      </c>
+      <c r="P3" s="90">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="90">
+        <v>0</v>
+      </c>
+      <c r="R3" s="90">
+        <v>0</v>
+      </c>
+      <c r="S3" s="90">
+        <v>0</v>
+      </c>
+      <c r="T3" s="90">
+        <v>0</v>
+      </c>
+      <c r="U3" s="90">
+        <v>0</v>
+      </c>
+      <c r="V3" s="90">
+        <v>0</v>
+      </c>
+      <c r="W3" s="90">
+        <v>0</v>
+      </c>
+      <c r="X3" s="90">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="90">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="90">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="90">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="90">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="90">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="90">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="90">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="90">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" ht="16.5">
+      <c r="A4" s="92" t="s">
+        <v>366</v>
+      </c>
+      <c r="B4" s="89">
+        <v>0</v>
+      </c>
+      <c r="C4" s="89">
+        <v>0</v>
+      </c>
+      <c r="D4" s="89">
+        <v>0</v>
+      </c>
+      <c r="E4" s="89">
+        <v>0</v>
+      </c>
+      <c r="F4" s="89">
+        <v>0</v>
+      </c>
+      <c r="G4" s="89">
+        <v>0</v>
+      </c>
+      <c r="H4" s="89">
+        <v>0</v>
+      </c>
+      <c r="I4" s="89">
+        <v>0</v>
+      </c>
+      <c r="J4" s="89">
+        <v>0</v>
+      </c>
+      <c r="K4" s="89">
+        <v>0</v>
+      </c>
+      <c r="L4" s="89">
+        <v>0</v>
+      </c>
+      <c r="M4" s="89">
+        <v>0</v>
+      </c>
+      <c r="N4" s="89">
+        <v>0</v>
+      </c>
+      <c r="O4" s="89">
+        <v>0</v>
+      </c>
+      <c r="P4" s="89">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="89">
+        <v>0</v>
+      </c>
+      <c r="R4" s="89">
+        <v>0</v>
+      </c>
+      <c r="S4" s="89">
+        <v>0</v>
+      </c>
+      <c r="T4" s="89">
+        <v>0</v>
+      </c>
+      <c r="U4" s="89">
+        <v>0</v>
+      </c>
+      <c r="V4" s="89">
+        <v>0</v>
+      </c>
+      <c r="W4" s="89">
+        <v>0</v>
+      </c>
+      <c r="X4" s="89">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="89">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="89">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="89">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="89">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="89">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="89">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="89">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="89">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" ht="16.5">
+      <c r="A5" s="94" t="s">
+        <v>367</v>
+      </c>
+      <c r="B5" s="95">
+        <v>0</v>
+      </c>
+      <c r="C5" s="95">
+        <v>0</v>
+      </c>
+      <c r="D5" s="95">
+        <v>0</v>
+      </c>
+      <c r="E5" s="95">
+        <v>0</v>
+      </c>
+      <c r="F5" s="95">
+        <v>0</v>
+      </c>
+      <c r="G5" s="95">
+        <v>0</v>
+      </c>
+      <c r="H5" s="95">
+        <v>0</v>
+      </c>
+      <c r="I5" s="95">
+        <v>0</v>
+      </c>
+      <c r="J5" s="95">
+        <v>0</v>
+      </c>
+      <c r="K5" s="95">
+        <v>0</v>
+      </c>
+      <c r="L5" s="95">
+        <v>0</v>
+      </c>
+      <c r="M5" s="95">
+        <v>0</v>
+      </c>
+      <c r="N5" s="95">
+        <v>0</v>
+      </c>
+      <c r="O5" s="95">
+        <v>0</v>
+      </c>
+      <c r="P5" s="95">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="95">
+        <v>0</v>
+      </c>
+      <c r="R5" s="95">
+        <v>0</v>
+      </c>
+      <c r="S5" s="95">
+        <v>0</v>
+      </c>
+      <c r="T5" s="95">
+        <v>0</v>
+      </c>
+      <c r="U5" s="95">
+        <v>0</v>
+      </c>
+      <c r="V5" s="95">
+        <v>0</v>
+      </c>
+      <c r="W5" s="95">
+        <v>0</v>
+      </c>
+      <c r="X5" s="95">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="95">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="95">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="95">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="95">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="95">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="95">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="95">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="95">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="95">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add s_logo in resource
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\GitHub\MSSeed13Camp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chelsea/Documents/Microsoft/領袖營/MSSeed13Camp/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="23100" windowHeight="15465" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23100" windowHeight="15460" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
     <sheet name="account" sheetId="2" r:id="rId2"/>
     <sheet name="resource" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="402">
   <si>
     <t>簡嘉誼</t>
   </si>
@@ -1242,15 +1242,18 @@
   <si>
     <t>led_light</t>
   </si>
+  <si>
+    <t>s_logo</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -3313,19 +3316,19 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="88" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" style="88" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="59.85546875" style="1" customWidth="1"/>
-    <col min="9" max="254" width="8.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="59.83203125" style="1" customWidth="1"/>
+    <col min="9" max="254" width="8.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="88" t="s">
         <v>361</v>
       </c>
@@ -3348,7 +3351,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="2" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="88">
         <v>1</v>
       </c>
@@ -3371,7 +3374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="88">
         <v>2</v>
       </c>
@@ -3394,7 +3397,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="88">
         <v>3</v>
       </c>
@@ -3417,7 +3420,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="5" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="88">
         <v>4</v>
       </c>
@@ -3440,7 +3443,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="88">
         <v>5</v>
       </c>
@@ -3463,7 +3466,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="7" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="88">
         <v>6</v>
       </c>
@@ -3486,7 +3489,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="8" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="88">
         <v>7</v>
       </c>
@@ -3509,7 +3512,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="9" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="88">
         <v>8</v>
       </c>
@@ -3532,7 +3535,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="10" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="88">
         <v>9</v>
       </c>
@@ -3555,7 +3558,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="11" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="88">
         <v>10</v>
       </c>
@@ -3578,7 +3581,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="12" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="88">
         <v>11</v>
       </c>
@@ -3601,7 +3604,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="13" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="88">
         <v>12</v>
       </c>
@@ -3624,7 +3627,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="88">
         <v>13</v>
       </c>
@@ -3647,7 +3650,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="15" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="88">
         <v>14</v>
       </c>
@@ -3670,7 +3673,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="16" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="88">
         <v>15</v>
       </c>
@@ -3693,7 +3696,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="17" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="88">
         <v>16</v>
       </c>
@@ -3716,7 +3719,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="18" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="88">
         <v>17</v>
       </c>
@@ -3739,7 +3742,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="19" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="88">
         <v>18</v>
       </c>
@@ -3762,7 +3765,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="20" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="88">
         <v>19</v>
       </c>
@@ -3785,7 +3788,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="21" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="88">
         <v>20</v>
       </c>
@@ -3808,7 +3811,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="22" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="88">
         <v>21</v>
       </c>
@@ -3831,7 +3834,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="23" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="88">
         <v>22</v>
       </c>
@@ -3852,7 +3855,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="24" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="88">
         <v>23</v>
       </c>
@@ -3875,7 +3878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="25" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="88">
         <v>24</v>
       </c>
@@ -3898,7 +3901,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="26" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="88">
         <v>25</v>
       </c>
@@ -3921,7 +3924,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="27" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="88">
         <v>26</v>
       </c>
@@ -3944,7 +3947,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="28" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="88">
         <v>27</v>
       </c>
@@ -3967,7 +3970,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="29" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="88">
         <v>28</v>
       </c>
@@ -3990,7 +3993,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="30" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="88">
         <v>29</v>
       </c>
@@ -4013,7 +4016,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="31" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="88">
         <v>30</v>
       </c>
@@ -4036,7 +4039,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="32" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="88">
         <v>31</v>
       </c>
@@ -4059,7 +4062,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="33" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="88">
         <v>32</v>
       </c>
@@ -4082,7 +4085,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="34" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="88">
         <v>33</v>
       </c>
@@ -4105,7 +4108,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="35" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="88">
         <v>34</v>
       </c>
@@ -4128,7 +4131,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="36" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="88">
         <v>35</v>
       </c>
@@ -4151,7 +4154,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="37" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="88">
         <v>36</v>
       </c>
@@ -4174,7 +4177,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="38" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="88">
         <v>37</v>
       </c>
@@ -4197,7 +4200,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="39" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="88">
         <v>38</v>
       </c>
@@ -4220,7 +4223,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="40" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="88">
         <v>39</v>
       </c>
@@ -4243,7 +4246,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="41" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="88">
         <v>40</v>
       </c>
@@ -4266,7 +4269,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="42" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="88">
         <v>41</v>
       </c>
@@ -4289,7 +4292,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="43" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="88">
         <v>42</v>
       </c>
@@ -4312,7 +4315,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="44" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="88">
         <v>43</v>
       </c>
@@ -4335,7 +4338,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="45" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="88">
         <v>44</v>
       </c>
@@ -4358,7 +4361,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="46" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="88">
         <v>45</v>
       </c>
@@ -4381,7 +4384,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="47" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="88">
         <v>46</v>
       </c>
@@ -4404,7 +4407,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="48" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="88">
         <v>47</v>
       </c>
@@ -4427,7 +4430,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="49" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="88">
         <v>48</v>
       </c>
@@ -4450,7 +4453,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="50" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="88">
         <v>49</v>
       </c>
@@ -4473,7 +4476,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="51" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="88">
         <v>50</v>
       </c>
@@ -4496,7 +4499,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="52" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="88">
         <v>51</v>
       </c>
@@ -4519,7 +4522,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="53" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="88">
         <v>52</v>
       </c>
@@ -4542,7 +4545,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="54" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="88">
         <v>53</v>
       </c>
@@ -4565,7 +4568,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="55" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="88">
         <v>54</v>
       </c>
@@ -4588,7 +4591,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="56" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="88">
         <v>55</v>
       </c>
@@ -4611,7 +4614,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="57" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="88">
         <v>56</v>
       </c>
@@ -4634,7 +4637,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="58" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="88">
         <v>57</v>
       </c>
@@ -4657,7 +4660,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="59" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="88">
         <v>58</v>
       </c>
@@ -4680,7 +4683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="60" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="88">
         <v>59</v>
       </c>
@@ -4703,7 +4706,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="61" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="88">
         <v>60</v>
       </c>
@@ -4726,7 +4729,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="62" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="88">
         <v>61</v>
       </c>
@@ -4749,7 +4752,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="63" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="88">
         <v>62</v>
       </c>
@@ -4772,7 +4775,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="64" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="88">
         <v>63</v>
       </c>
@@ -4795,7 +4798,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="65" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="88">
         <v>64</v>
       </c>
@@ -4818,7 +4821,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="66" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="88">
         <v>65</v>
       </c>
@@ -4841,7 +4844,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="67" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="88">
         <v>66</v>
       </c>
@@ -4862,7 +4865,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="68" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="88">
         <v>67</v>
       </c>
@@ -4885,7 +4888,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="69" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="88">
         <v>68</v>
       </c>
@@ -4908,7 +4911,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="70" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="88">
         <v>69</v>
       </c>
@@ -4931,7 +4934,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="71" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="88">
         <v>70</v>
       </c>
@@ -4954,7 +4957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="72" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="88">
         <v>71</v>
       </c>
@@ -4977,7 +4980,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="73" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="88">
         <v>72</v>
       </c>
@@ -5000,7 +5003,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="74" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="88">
         <v>73</v>
       </c>
@@ -5023,7 +5026,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="75" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="88">
         <v>74</v>
       </c>
@@ -5046,7 +5049,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="76" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="88">
         <v>75</v>
       </c>
@@ -5067,7 +5070,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="77" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="88">
         <v>76</v>
       </c>
@@ -5090,7 +5093,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="78" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="88">
         <v>77</v>
       </c>
@@ -5113,7 +5116,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="79" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="88">
         <v>78</v>
       </c>
@@ -5136,7 +5139,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="80" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="88">
         <v>79</v>
       </c>
@@ -5159,7 +5162,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="81" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="88">
         <v>80</v>
       </c>
@@ -5182,7 +5185,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="82" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="88">
         <v>81</v>
       </c>
@@ -5205,7 +5208,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="83" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="88">
         <v>82</v>
       </c>
@@ -5228,7 +5231,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="84" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="88">
         <v>83</v>
       </c>
@@ -5251,7 +5254,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="85" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="88">
         <v>84</v>
       </c>
@@ -5274,7 +5277,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="86" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="88">
         <v>85</v>
       </c>
@@ -5297,7 +5300,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="87" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="88">
         <v>86</v>
       </c>
@@ -5320,7 +5323,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="88" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="88">
         <v>87</v>
       </c>
@@ -5343,7 +5346,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="89" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="88">
         <v>88</v>
       </c>
@@ -5366,7 +5369,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="90" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="88">
         <v>89</v>
       </c>
@@ -5389,7 +5392,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="91" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="88">
         <v>90</v>
       </c>
@@ -5412,7 +5415,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="92" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="88">
         <v>91</v>
       </c>
@@ -5435,7 +5438,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="93" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="88">
         <v>92</v>
       </c>
@@ -5458,7 +5461,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="94" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="88">
         <v>93</v>
       </c>
@@ -5481,7 +5484,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="95" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="88">
         <v>94</v>
       </c>
@@ -5504,7 +5507,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="96" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="88">
         <v>95</v>
       </c>
@@ -5527,7 +5530,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="97" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="88">
         <v>96</v>
       </c>
@@ -5550,7 +5553,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="98" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="88">
         <v>97</v>
       </c>
@@ -5573,7 +5576,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="99" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="88">
         <v>98</v>
       </c>
@@ -5596,7 +5599,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="100" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="88">
         <v>99</v>
       </c>
@@ -5619,7 +5622,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="101" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="88">
         <v>100</v>
       </c>
@@ -5642,7 +5645,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="102" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="88">
         <v>101</v>
       </c>
@@ -5665,7 +5668,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="103" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="88">
         <v>102</v>
       </c>
@@ -5688,7 +5691,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="104" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="88">
         <v>103</v>
       </c>
@@ -5711,7 +5714,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="105" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="88">
         <v>104</v>
       </c>
@@ -5756,13 +5759,13 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="88"/>
-    <col min="2" max="2" width="59.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="88"/>
+    <col min="2" max="2" width="59.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="88" t="s">
         <v>348</v>
       </c>
@@ -5773,7 +5776,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.25">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="88">
         <v>1</v>
       </c>
@@ -5784,7 +5787,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.25">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="88">
         <v>2</v>
       </c>
@@ -5792,7 +5795,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.25">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="88">
         <v>3</v>
       </c>
@@ -5800,7 +5803,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.25">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="88">
         <v>4</v>
       </c>
@@ -5808,7 +5811,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17.25">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="88">
         <v>5</v>
       </c>
@@ -5816,7 +5819,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17.25">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="88">
         <v>6</v>
       </c>
@@ -5824,7 +5827,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17.25">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="88">
         <v>7</v>
       </c>
@@ -5832,7 +5835,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.25">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="88">
         <v>8</v>
       </c>
@@ -5840,7 +5843,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.25">
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="88">
         <v>9</v>
       </c>
@@ -5848,7 +5851,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.25">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="88">
         <v>10</v>
       </c>
@@ -5856,7 +5859,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="88">
         <v>11</v>
       </c>
@@ -5864,7 +5867,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.25">
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="88">
         <v>12</v>
       </c>
@@ -5872,7 +5875,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17.25">
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="88">
         <v>13</v>
       </c>
@@ -5880,7 +5883,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17.25">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="88">
         <v>14</v>
       </c>
@@ -5888,7 +5891,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17.25">
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="88">
         <v>15</v>
       </c>
@@ -5896,7 +5899,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="17.25">
+    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="88">
         <v>16</v>
       </c>
@@ -5904,7 +5907,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="17.25">
+    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="88">
         <v>17</v>
       </c>
@@ -5912,7 +5915,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="17.25">
+    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="88">
         <v>18</v>
       </c>
@@ -5920,7 +5923,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="17.25">
+    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="88">
         <v>19</v>
       </c>
@@ -5928,7 +5931,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="17.25">
+    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="88">
         <v>20</v>
       </c>
@@ -5936,7 +5939,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="17.25">
+    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="88">
         <v>21</v>
       </c>
@@ -5944,7 +5947,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="17.25">
+    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="88">
         <v>22</v>
       </c>
@@ -5952,7 +5955,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="17.25">
+    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="88">
         <v>23</v>
       </c>
@@ -5960,7 +5963,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="17.25">
+    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="88">
         <v>24</v>
       </c>
@@ -5968,7 +5971,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="17.25">
+    <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="88">
         <v>25</v>
       </c>
@@ -5976,7 +5979,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="17.25">
+    <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="88">
         <v>26</v>
       </c>
@@ -5984,7 +5987,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="17.25">
+    <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="88">
         <v>27</v>
       </c>
@@ -5992,7 +5995,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="17.25">
+    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="88">
         <v>28</v>
       </c>
@@ -6000,7 +6003,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="17.25">
+    <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="88">
         <v>29</v>
       </c>
@@ -6008,7 +6011,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="17.25">
+    <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="88">
         <v>30</v>
       </c>
@@ -6016,7 +6019,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="17.25">
+    <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="88">
         <v>31</v>
       </c>
@@ -6024,7 +6027,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="17.25">
+    <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="88">
         <v>32</v>
       </c>
@@ -6032,7 +6035,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="17.25">
+    <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="88">
         <v>33</v>
       </c>
@@ -6040,7 +6043,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="17.25">
+    <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="88">
         <v>34</v>
       </c>
@@ -6048,7 +6051,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="17.25">
+    <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="88">
         <v>35</v>
       </c>
@@ -6056,7 +6059,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="17.25">
+    <row r="37" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="88">
         <v>36</v>
       </c>
@@ -6064,7 +6067,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="17.25">
+    <row r="38" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="88">
         <v>37</v>
       </c>
@@ -6072,7 +6075,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="17.25">
+    <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="88">
         <v>38</v>
       </c>
@@ -6080,7 +6083,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="17.25">
+    <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="88">
         <v>39</v>
       </c>
@@ -6088,7 +6091,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="17.25">
+    <row r="41" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="88">
         <v>40</v>
       </c>
@@ -6096,7 +6099,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="17.25">
+    <row r="42" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="88">
         <v>41</v>
       </c>
@@ -6104,7 +6107,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="17.25">
+    <row r="43" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="88">
         <v>42</v>
       </c>
@@ -6112,7 +6115,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="17.25">
+    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="88">
         <v>43</v>
       </c>
@@ -6120,7 +6123,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="17.25">
+    <row r="45" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="88">
         <v>44</v>
       </c>
@@ -6128,7 +6131,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="17.25">
+    <row r="46" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="88">
         <v>45</v>
       </c>
@@ -6136,7 +6139,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="17.25">
+    <row r="47" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="88">
         <v>46</v>
       </c>
@@ -6144,7 +6147,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="17.25">
+    <row r="48" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="88">
         <v>47</v>
       </c>
@@ -6152,7 +6155,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="17.25">
+    <row r="49" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="88">
         <v>48</v>
       </c>
@@ -6160,7 +6163,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="17.25">
+    <row r="50" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="88">
         <v>49</v>
       </c>
@@ -6168,7 +6171,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="17.25">
+    <row r="51" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="88">
         <v>50</v>
       </c>
@@ -6176,7 +6179,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="17.25">
+    <row r="52" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="88">
         <v>51</v>
       </c>
@@ -6184,7 +6187,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="17.25">
+    <row r="53" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="88">
         <v>52</v>
       </c>
@@ -6192,7 +6195,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="17.25">
+    <row r="54" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="88">
         <v>53</v>
       </c>
@@ -6200,7 +6203,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="17.25">
+    <row r="55" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="88">
         <v>54</v>
       </c>
@@ -6208,7 +6211,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="17.25">
+    <row r="56" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="88">
         <v>55</v>
       </c>
@@ -6216,7 +6219,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="17.25">
+    <row r="57" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="88">
         <v>56</v>
       </c>
@@ -6224,7 +6227,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="17.25">
+    <row r="58" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="88">
         <v>57</v>
       </c>
@@ -6232,7 +6235,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="17.25">
+    <row r="59" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="88">
         <v>58</v>
       </c>
@@ -6240,7 +6243,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="17.25">
+    <row r="60" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="88">
         <v>59</v>
       </c>
@@ -6248,7 +6251,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="17.25">
+    <row r="61" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="88">
         <v>60</v>
       </c>
@@ -6256,7 +6259,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="17.25">
+    <row r="62" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="88">
         <v>61</v>
       </c>
@@ -6264,7 +6267,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="88">
         <v>62</v>
       </c>
@@ -6272,7 +6275,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="17.25">
+    <row r="64" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="88">
         <v>63</v>
       </c>
@@ -6280,7 +6283,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="17.25">
+    <row r="65" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="88">
         <v>64</v>
       </c>
@@ -6288,7 +6291,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="17.25">
+    <row r="66" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="88">
         <v>65</v>
       </c>
@@ -6296,7 +6299,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="17.25">
+    <row r="67" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="88">
         <v>66</v>
       </c>
@@ -6304,7 +6307,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="17.25">
+    <row r="68" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="88">
         <v>67</v>
       </c>
@@ -6312,7 +6315,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="17.25">
+    <row r="69" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="88">
         <v>68</v>
       </c>
@@ -6320,7 +6323,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="17.25">
+    <row r="70" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="88">
         <v>69</v>
       </c>
@@ -6328,7 +6331,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="17.25">
+    <row r="71" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="88">
         <v>70</v>
       </c>
@@ -6336,7 +6339,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="17.25">
+    <row r="72" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="88">
         <v>71</v>
       </c>
@@ -6344,7 +6347,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="17.25">
+    <row r="73" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="88">
         <v>72</v>
       </c>
@@ -6352,7 +6355,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="17.25">
+    <row r="74" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="88">
         <v>73</v>
       </c>
@@ -6360,7 +6363,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="17.25">
+    <row r="75" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="88">
         <v>74</v>
       </c>
@@ -6368,13 +6371,13 @@
         <v>257</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="17.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="88">
         <v>75</v>
       </c>
       <c r="B76" s="29"/>
     </row>
-    <row r="77" spans="1:2" ht="17.25">
+    <row r="77" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="88">
         <v>76</v>
       </c>
@@ -6382,7 +6385,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="17.25">
+    <row r="78" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="88">
         <v>77</v>
       </c>
@@ -6390,7 +6393,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="17.25">
+    <row r="79" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="88">
         <v>78</v>
       </c>
@@ -6398,7 +6401,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="17.25">
+    <row r="80" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="88">
         <v>79</v>
       </c>
@@ -6406,7 +6409,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="17.25">
+    <row r="81" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="88">
         <v>80</v>
       </c>
@@ -6414,7 +6417,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="17.25">
+    <row r="82" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="88">
         <v>81</v>
       </c>
@@ -6422,7 +6425,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="17.25">
+    <row r="83" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="88">
         <v>82</v>
       </c>
@@ -6430,7 +6433,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="17.25">
+    <row r="84" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="88">
         <v>83</v>
       </c>
@@ -6438,7 +6441,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="17.25">
+    <row r="85" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="88">
         <v>84</v>
       </c>
@@ -6446,7 +6449,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="17.25">
+    <row r="86" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="88">
         <v>85</v>
       </c>
@@ -6454,7 +6457,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="17.25">
+    <row r="87" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="88">
         <v>86</v>
       </c>
@@ -6462,7 +6465,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="17.25">
+    <row r="88" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="88">
         <v>87</v>
       </c>
@@ -6470,7 +6473,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="17.25">
+    <row r="89" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="88">
         <v>88</v>
       </c>
@@ -6478,7 +6481,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="17.25">
+    <row r="90" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="88">
         <v>89</v>
       </c>
@@ -6486,7 +6489,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="17.25">
+    <row r="91" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="88">
         <v>90</v>
       </c>
@@ -6494,7 +6497,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="17.25">
+    <row r="92" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="88">
         <v>91</v>
       </c>
@@ -6502,7 +6505,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="17.25">
+    <row r="93" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="88">
         <v>92</v>
       </c>
@@ -6510,7 +6513,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="17.25">
+    <row r="94" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="88">
         <v>93</v>
       </c>
@@ -6518,7 +6521,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="17.25">
+    <row r="95" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="88">
         <v>94</v>
       </c>
@@ -6526,7 +6529,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="17.25">
+    <row r="96" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="88">
         <v>95</v>
       </c>
@@ -6534,7 +6537,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="17.25">
+    <row r="97" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="88">
         <v>96</v>
       </c>
@@ -6542,7 +6545,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="17.25">
+    <row r="98" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="88">
         <v>97</v>
       </c>
@@ -6550,7 +6553,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="17.25">
+    <row r="99" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="88">
         <v>98</v>
       </c>
@@ -6558,7 +6561,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="17.25">
+    <row r="100" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="88">
         <v>99</v>
       </c>
@@ -6566,7 +6569,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="17.25">
+    <row r="101" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="88">
         <v>100</v>
       </c>
@@ -6574,7 +6577,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="17.25">
+    <row r="102" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="88">
         <v>101</v>
       </c>
@@ -6582,7 +6585,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="17.25">
+    <row r="103" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="88">
         <v>102</v>
       </c>
@@ -6590,7 +6593,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="17.25">
+    <row r="104" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="88">
         <v>103</v>
       </c>
@@ -6598,7 +6601,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="17.25">
+    <row r="105" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="88">
         <v>104</v>
       </c>
@@ -6616,48 +6619,49 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG5"/>
+  <dimension ref="A1:AH5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD10" sqref="AD10"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AJ21" sqref="AJ21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="2.83203125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.6640625" customWidth="1"/>
+    <col min="30" max="30" width="6" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="24.75">
+    <row r="1" spans="1:34" ht="37" x14ac:dyDescent="0.2">
       <c r="A1" s="91" t="s">
         <v>368</v>
       </c>
@@ -6742,124 +6746,130 @@
       <c r="AB1" s="96" t="s">
         <v>395</v>
       </c>
-      <c r="AC1" s="97" t="s">
+      <c r="AC1" s="96" t="s">
+        <v>401</v>
+      </c>
+      <c r="AD1" s="97" t="s">
         <v>396</v>
       </c>
-      <c r="AD1" s="96" t="s">
+      <c r="AE1" s="96" t="s">
         <v>397</v>
       </c>
-      <c r="AE1" s="97" t="s">
+      <c r="AF1" s="97" t="s">
         <v>398</v>
       </c>
-      <c r="AF1" s="96" t="s">
+      <c r="AG1" s="96" t="s">
         <v>399</v>
       </c>
-      <c r="AG1" s="98" t="s">
+      <c r="AH1" s="98" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="16.5">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" s="92" t="s">
         <v>364</v>
       </c>
       <c r="B2" s="89">
+        <v>1</v>
+      </c>
+      <c r="C2" s="89">
+        <v>2</v>
+      </c>
+      <c r="D2" s="89">
+        <v>3</v>
+      </c>
+      <c r="E2" s="89">
+        <v>4</v>
+      </c>
+      <c r="F2" s="89">
+        <v>5</v>
+      </c>
+      <c r="G2" s="89">
+        <v>6</v>
+      </c>
+      <c r="H2" s="89">
+        <v>7</v>
+      </c>
+      <c r="I2" s="89">
+        <v>8</v>
+      </c>
+      <c r="J2" s="89">
+        <v>9</v>
+      </c>
+      <c r="K2" s="89">
         <v>10</v>
       </c>
-      <c r="C2" s="89">
-        <v>7</v>
-      </c>
-      <c r="D2" s="89">
-        <v>0</v>
-      </c>
-      <c r="E2" s="89">
-        <v>0</v>
-      </c>
-      <c r="F2" s="89">
-        <v>0</v>
-      </c>
-      <c r="G2" s="89">
-        <v>0</v>
-      </c>
-      <c r="H2" s="89">
-        <v>0</v>
-      </c>
-      <c r="I2" s="89">
-        <v>0</v>
-      </c>
-      <c r="J2" s="89">
-        <v>0</v>
-      </c>
-      <c r="K2" s="89">
-        <v>0</v>
-      </c>
       <c r="L2" s="89">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="M2" s="89">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="N2" s="89">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="O2" s="89">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P2" s="89">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Q2" s="89">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R2" s="89">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="S2" s="89">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="T2" s="89">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="U2" s="89">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="V2" s="89">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="W2" s="89">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="X2" s="89">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="Y2" s="89">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Z2" s="89">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AA2" s="89">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AB2" s="89">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AC2" s="89">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AD2" s="89">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AE2" s="89">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AF2" s="89">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="AG2" s="89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" ht="16.5">
+        <v>32</v>
+      </c>
+      <c r="AH2" s="89">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" s="93" t="s">
         <v>365</v>
       </c>
@@ -6959,8 +6969,11 @@
       <c r="AG3" s="90">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:33" ht="16.5">
+      <c r="AH3" s="90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" s="92" t="s">
         <v>366</v>
       </c>
@@ -7060,8 +7073,11 @@
       <c r="AG4" s="89">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" ht="16.5">
+      <c r="AH4" s="89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="94" t="s">
         <v>367</v>
       </c>
@@ -7159,6 +7175,9 @@
         <v>0</v>
       </c>
       <c r="AG5" s="95">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="95">
         <v>0</v>
       </c>
     </row>

</xml_diff>